<commit_message>
fixed last column in dataframe output and added more words to cloud
</commit_message>
<xml_diff>
--- a/job_data.xlsx
+++ b/job_data.xlsx
@@ -512,7 +512,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>(('have', 16),)</t>
+          <t>['have', 'deliver', 'work', 'drive', 'help', 'connect', 'support', 'know', 'build', 'bring', 'leverage', 'focus', 'manage', 'root', 'want', 'own', 'create', 'transform', 'interact', 'lead', 'oversee', 'do', 'enable', 'solutionsmarkete', 'solve', 'sell', 'expect', 'suit', 'make', 'allow', 'understand', 'matter', 'respond', 'unlock', 'empower', 'respect', 'give', 'personalize', 'seek', 'elevate', 'set', 'end', 'automate', 'decisione', 'ensure', 'meet', 'include', 'continue', 'pay', 'mentor', 'join', 'grow', 'maintain', 'structure', 'align', 'engage', 'inspire', 'act', 'implement', 'operate', 'market', 'serve', 'follow', 'operationsadvertise', 'base', 'accelerate', 'resultsqualificationsrequire', 'bringyou', 'develop', 'expand', 'kpi', 'provide', 'learn', 'improve', 'take', 'pull', 'demonstrate', 'staff', 'achieve', 'position', 'triage', 'prioritize', 'compete', 'pace', 'prove', 'produce', 'write', 'authorize', 'travel', 'suspend', 'vary']</t>
         </is>
       </c>
     </row>
@@ -553,7 +553,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>(('deliver', 10),)</t>
+          <t>['work', 'drive', 'lead', 'solve', 'take', 'provide', 'prioritize', 'communicate', 'manage', 'relate', 'integrate', 'address', 'cross', 'responsibilitiesidentify', 'benefit', 'validate', 'utilize', 'review', 'models.contribute', 'feature', 'help', 'scope', 'timeline', 'deal', 'deliver', 'enable', 'scale', 'define', 'create', 'compete', 'translate', 'technologiesoutstande', 'do', 'follow', 'perform', 'impact', 'develop', 'implement', 'preferred.applie', 'boost', 'inspire', 'maximize', 'dig', 'think', 'pace', 'break', 'defend', 'debate', 'use', 'base']</t>
         </is>
       </c>
     </row>
@@ -594,7 +594,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>(('work', 7),)</t>
+          <t>['identify', 'include', 'build', 'work', 'improve', 'communicate', 'seek', 'use', 'apply', 'solve', 'drive', 'protect', 'support', 'become', 'develop', 'increase', 'provide', 'grow', 'analyze', 'automate', 'innovate', 'look', 'desire', 'model', 'discover', 'cut', 'design', 'answer', 'resolution', 'define', 'deliver', 'unlock', 'detect', 'source', 'conduct', 'query', 'offline', 'casescollaborate', 'enhance', 'understand', 'know', 'use.maintain', 'diverse', 'presentationsabout', 'leverage', 'make', 'effortless', 'relate', 'script', 'write', 'present', 'datapreferre', 'demonstrate', 'exceed', 'prioritize', 'sacrifice', 'dive', 'commit', 'discriminate', 'like', 'request', 'visit', 'a1985797']</t>
         </is>
       </c>
     </row>
@@ -635,7 +635,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>(('drive', 5),)</t>
+          <t>['require', 'include', 'learn', 'leverage', 'develop', 'validate', 'communicate', 'make', 'receive', 'need', 'follow', 'provide', 'allow', 'commit', 'set', 'evaluate', 'understand', 'regard', 'establish', 'procedures.require', 'relate', 'toolsexperience', 'solve', 'write', 'work', 'contribute', 'focus', 'improve', 'associate', 'have', 'lack', 'protect', 'informationpreferre', 'manage', 'perform', 'build', 'covid', 'undergo', 'wear', 'cover', 'do', 'approve', 'come', 'put', 'progress', 'offer', 'test', 'support', 'use', 'interview', 'call', 'enhance', 'connect', 'gain', 'pertain', 'select', 'check', 'ensure', 'miss', 'invite', 'participate', 'listen', 'anticipate', 'take', 'review', 'inform', 'move', 'interviews.schedule']</t>
         </is>
       </c>
     </row>
@@ -676,7 +676,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>(('help', 5),)</t>
+          <t>['build', 'solve', 'apply', 'learn', '’re', 'advance', 'obsess', 'make', 'change', 'consume', 'partner', 'lead', 'transform', 'use', 'excite', 'love', 'hear', 'teamarchitect', 'underlie', 'package', 'do', 'work', 'challenge', 'visionocrhandwrite', 'languagefinde', 'contractsextracte', 'clusteringworke', 'require', 'follow', 'academia', 'relate', 'discriminate', 'protect', 'include']</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>(('connect', 5),)</t>
+          <t>['go', 'do', 'use', 'need', 'patch', 'look', 'get', 'enhance', 'have', 'complete', 'realize', 'propose', 'include', 'figure', 'impact', 'categorize', 'join', 'unite', 'share', 'make', 'discover', 'personalize', 'provide', 'consist', 'develop', 'purchase', 'ecosystemfacilitate', 'take', 'check', 'route', 'send', 'own', 'bridge', 'turn', 'prioritize', 'contribute', 'put', 'start', 'create', 'identify', 'tour', 'observe', 'exist', 'assist', 'come', 'includeworke', 'talk', 'schedule', 'happen', 'miss', 'coordinate', 'be', 'imagine', 'speak', 'reach', 'internshipbee', 'orient', 'organize', 'pull', 'involve', 'enrol', 'major', 'demonstrate', '’s', 'work', 'establish', 'explore', 'implement', 'invite', 'participate', 'network', 'encourage', 'bear', 'discriminate', 'protect', 'prohibit']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add updated file output
</commit_message>
<xml_diff>
--- a/job_data.xlsx
+++ b/job_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -609,33 +609,33 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Cognitive/Machine Learning Professional II</t>
+          <t>SWE, Machine Learning (ML)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Humana</t>
+          <t>Instabase</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>r-276898descriptionthe cognitive/machine learning professional ii leverages large sets of structured and unstructured data to develop tactical and strategic insights. the cognitive/machine learning professional ii work assignments are varied and frequently require interpretation and independent determination of the appropriate courses of action.responsibilitiesthe cognitive/machine learning professional ii collaborates with analytic and data teams to set objectives, approaches, and work plans. researches and evaluates new analytical methodologies, approaches, and solutions. develops and validates statistical forecasting models and tools. interprets and communicates analytic results to analytical and non-analytical business partners and executive decision makers. understands department, segment, and organizational strategy and operating objectives, including their linkages to related areas. makes decisions regarding own work methods, occasionally in ambiguous situations, and requires minimal direction and receives guidance where needed. follows established guidelines/procedures.required qualificationsbachelor's degree in a quantitative discipline, such as computer science, econometrics, mathematics and/or related fieldminimum 3 years of professional experience leveraging large sets of structured and unstructured data to develop tactical and strategic insightsexperience developing and validating statistical forecasting models and toolsexperience interpreting and communicating analytic results to analytical and non-analytical business partners and executive decision makersexperience leveraging data science techniques to solve problemsclear oral and written communication skillsflexible, dynamic personality who is able to work independently in a team environmentproficient in both sql and python programming languagesmust be passionate about contributing to an organization focused on continuously improving consumer experiencesmust be available for core business hours associated with eastern time zonework-at-home requirementswah requirements: must have the ability to provide a high speed dsl or cable modem for a home office (satellite and wireless internet service is not allowed for this role). a minimum standard speed for optimal performance of 25x10 (25mpbs download x 10mpbs upload) is required.a dedicated space lacking ongoing interruptions to protect member phi / hipaa informationpreferred qualificationshealthcare or managed care experienceexperience performing data management, mining, and manipulation along with analyticsexperience in etl techniques for building data sets for modelscovid-19 vaccine policyfor this job, associates are required to be fully covid vaccinated, including booster or undergo weekly covid testing and wear a face covering while at work. the weekly testing will need to be done through an approved humana vendor, and unvaccinated associates should follow all social distancing and masking protocols if they are required to come into a humana facility or work outside of their home. we are a healthcare company committed to putting health and safety first for our members, patients, associates, and the communities we serve.if progressed to offer, you will be required toprovide proof of full vaccination, including booster or commit to testing protocols orprovide proof of applicable exemption including any required supporting documentationmedical, religious, state and remote-only work exemptions are available.additional informationas part of our hiring process for this opportunity, we will be using an exciting interviewing technology called modern hire to enhance our hiring and decision-making ability. modern hire allows us to quickly connect and gain valuable information from you pertaining to your relevant skills and experience at a time that is best for your schedule. if you are selected for a first round interview, you will receive an email correspondence (please be sure to check your spam or junk folders often to ensure communication isn’t missed) inviting you to participate in a modern hire interview. in this interview, you will listen to a set of interview questions over your phone and you will provide recorded responses to each question. you should anticipate this interview to take about 15 to 30 minutes. your recorded interview will be reviewed and you will subsequently be informed if you will be moving forward to next round of interviews.scheduled weekly hours40</t>
+          <t>at instabase, we’re passionate about building software to advance the state of the art in computing. we’ve built a fearlessly experimental, customer-obsessed team who are making discoveries to fundamentally change how people build and consume business applications. today, we’re partnering with the world’s leading companies to transform how they use data and technology. if these challenges excite you, we’d love to hear from you!our engineering teamarchitects the underlying operating system, core services, platform infrastructure, dev toolkits, core algorithms, machine learning models, packaged end-user apps, and app store marketplace. instabase engineers are excited to solve hard problems for complex organizations and are self-starters from day one.what you will do:work on a small team of ml engineers to apply machine learning techniques to challenging real world problems such asimage processing / computer visionocrhandwriting recognitionvisual extraction (checkboxes, signatures, radio button, etc.)object detectiontable detectiondocument/text understandingextraction from documentsfield extraction from document with variable structure (for example: paystubs, invoices, forms, etc.)information retrieval from documents with natural languagefinding relevant clause in legal contractsextracting data (for example: effective date, duration, payment terms, etc.) from legal contractsdocument classificationdocument clusteringworking in this area require knowledge in one or more of the following:ms in computer science, engineering, math, science or related field. phd preferred.5+ years industry / academia experienceproven ttrack record of excellence in applying machine learning techniques for solving difficult real world problemsknowledge of deep learning frameworks such as pytorch and tensorflow, computer vision, nlp, or related areas would be a plus.instabase is an equal opportunity employer and values diversity in all forms. instabase does not discriminate on the basis of race, religion, color, national origin, gender identity, sexual orientation, age, marital status, protected veteran status, disability, or any other unlawful factor. instabase also complies with local laws, including the san francisco fair chance ordinance.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>r-276898descriptionthe cognitive/machine learning professional ii leverages large sets of structured and unstructured data to develop tactical and strategic insights. the cognitive/machine learning professional ii work assignments are varied and frequently require interpretation and independent determination of the appropriate courses of action.responsibilitiesthe cognitive/machine learning professional ii collaborates with analytic and data teams to set objectives, approaches, and work plans. researches and evaluates new analytical methodologies, approaches, and solutions. develops and validates statistical forecasting models and tools. interprets and communicates analytic results to analytical and non-analytical business partners and executive decision makers. understands department, segment, and organizational strategy and operating objectives, including their linkages to related areas. makes decisions regarding own work methods, occasionally in ambiguous situations, and requires minimal direction and receives guidance where needed. follows established guidelines/procedures.required qualificationsbachelor's degree in a quantitative discipline, such as computer science, econometrics, mathematics and/or related fieldminimum 3 years of professional experience leveraging large sets of structured and unstructured data to develop tactical and strategic insightsexperience developing and validating statistical forecasting models and toolsexperience interpreting and communicating analytic results to analytical and non-analytical business partners and executive decision makersexperience leveraging data science techniques to solve problemsclear oral and written communication skillsflexible, dynamic personality who is able to work independently in a team environmentproficient in both sql and python programming languagesmust be passionate about contributing to an organization focused on continuously improving consumer experiencesmust be available for core business hours associated with eastern time zonework-at-home requirementswah requirements: must have the ability to provide a high speed dsl or cable modem for a home office (satellite and wireless internet service is not allowed for this role). a minimum standard speed for optimal performance of 25x10 (25mpbs download x 10mpbs upload) is required.a dedicated space lacking ongoing interruptions to protect member phi / hipaa informationpreferred qualificationshealthcare or managed care experienceexperience performing data management, mining, and manipulation along with analyticsexperience in etl techniques for building data sets for modelscovid-19 vaccine policyfor this job, associates are required to be fully covid vaccinated, including booster or undergo weekly covid testing and wear a face covering while at work. the weekly testing will need to be done through an approved humana vendor, and unvaccinated associates should follow all social distancing and masking protocols if they are required to come into a humana facility or work outside of their home. we are a healthcare company committed to putting health and safety first for our members, patients, associates, and the communities we serve.if progressed to offer, you will be required toprovide proof of full vaccination, including booster or commit to testing protocols orprovide proof of applicable exemption including any required supporting documentationmedical, religious, state and remote-only work exemptions are available.additional informationas part of our hiring process for this opportunity, we will be using an exciting interviewing technology called modern hire to enhance our hiring and decision-making ability. modern hire allows us to quickly connect and gain valuable information from you pertaining to your relevant skills and experience at a time that is best for your schedule. if you are selected for a first round interview, you will receive an email correspondence (please be sure to check your spam or junk folders often to ensure communication isn’t missed) inviting you to participate in a modern hire interview. in this interview, you will listen to a set of interview questions over your phone and you will provide recorded responses to each question. you should anticipate this interview to take about 15 to 30 minutes. your recorded interview will be reviewed and you will subsequently be informed if you will be moving forward to next round of interviews.scheduled weekly hours40</t>
+          <t>at instabase, we’re passionate about building software to advance the state of the art in computing. we’ve built a fearlessly experimental, customer-obsessed team who are making discoveries to fundamentally change how people build and consume business applications. today, we’re partnering with the world’s leading companies to transform how they use data and technology. if these challenges excite you, we’d love to hear from you!our engineering teamarchitects the underlying operating system, core services, platform infrastructure, dev toolkits, core algorithms, machine learning models, packaged end-user apps, and app store marketplace. instabase engineers are excited to solve hard problems for complex organizations and are self-starters from day one.what you will do:work on a small team of ml engineers to apply machine learning techniques to challenging real world problems such asimage processing / computer visionocrhandwriting recognitionvisual extraction (checkboxes, signatures, radio button, etc.)object detectiontable detectiondocument/text understandingextraction from documentsfield extraction from document with variable structure (for example: paystubs, invoices, forms, etc.)information retrieval from documents with natural languagefinding relevant clause in legal contractsextracting data (for example: effective date, duration, payment terms, etc.) from legal contractsdocument classificationdocument clusteringworking in this area require knowledge in one or more of the following:ms in computer science, engineering, math, science or related field. phd preferred.5+ years industry / academia experienceproven ttrack record of excellence in applying machine learning techniques for solving difficult real world problemsknowledge of deep learning frameworks such as pytorch and tensorflow, computer vision, nlp, or related areas would be a plus.instabase is an equal opportunity employer and values diversity in all forms. instabase does not discriminate on the basis of race, religion, color, national origin, gender identity, sexual orientation, age, marital status, protected veteran status, disability, or any other unlawful factor. instabase also complies with local laws, including the san francisco fair chance ordinance.</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>0.1652762317048032</v>
+        <v>0.1270833333333334</v>
       </c>
       <c r="H5" t="n">
-        <v>0.3652518381089812</v>
+        <v>0.5035714285714287</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>['require', 'include', 'learn', 'leverage', 'develop', 'validate', 'communicate', 'make', 'receive', 'need', 'follow', 'provide', 'allow', 'commit', 'set', 'evaluate', 'understand', 'regard', 'establish', 'procedures.require', 'relate', 'toolsexperience', 'solve', 'write', 'work', 'contribute', 'focus', 'improve', 'associate', 'have', 'lack', 'protect', 'informationpreferre', 'manage', 'perform', 'build', 'covid', 'undergo', 'wear', 'cover', 'do', 'approve', 'come', 'put', 'progress', 'offer', 'test', 'support', 'use', 'interview', 'call', 'enhance', 'connect', 'gain', 'pertain', 'select', 'check', 'ensure', 'miss', 'invite', 'participate', 'listen', 'anticipate', 'take', 'review', 'inform', 'move', 'interviews.schedule']</t>
+          <t>['build', 'solve', 'apply', 'learn', '’re', 'advance', 'obsess', 'make', 'change', 'consume', 'partner', 'lead', 'transform', 'use', 'excite', 'love', 'hear', 'teamarchitect', 'underlie', 'package', 'do', 'work', 'challenge', 'visionocrhandwrite', 'languagefinde', 'contractsextracte', 'clusteringworke', 'require', 'follow', 'academia', 'relate', 'discriminate', 'protect', 'include']</t>
         </is>
       </c>
     </row>
@@ -650,72 +650,31 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>SWE, Machine Learning (ML)</t>
+          <t>Global Reference Lab Information Systems Intern</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Instabase</t>
+          <t>IDEXX</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>at instabase, we’re passionate about building software to advance the state of the art in computing. we’ve built a fearlessly experimental, customer-obsessed team who are making discoveries to fundamentally change how people build and consume business applications. today, we’re partnering with the world’s leading companies to transform how they use data and technology. if these challenges excite you, we’d love to hear from you!our engineering teamarchitects the underlying operating system, core services, platform infrastructure, dev toolkits, core algorithms, machine learning models, packaged end-user apps, and app store marketplace. instabase engineers are excited to solve hard problems for complex organizations and are self-starters from day one.what you will do:work on a small team of ml engineers to apply machine learning techniques to challenging real world problems such asimage processing / computer visionocrhandwriting recognitionvisual extraction (checkboxes, signatures, radio button, etc.)object detectiontable detectiondocument/text understandingextraction from documentsfield extraction from document with variable structure (for example: paystubs, invoices, forms, etc.)information retrieval from documents with natural languagefinding relevant clause in legal contractsextracting data (for example: effective date, duration, payment terms, etc.) from legal contractsdocument classificationdocument clusteringworking in this area require knowledge in one or more of the following:ms in computer science, engineering, math, science or related field. phd preferred.5+ years industry / academia experienceproven ttrack record of excellence in applying machine learning techniques for solving difficult real world problemsknowledge of deep learning frameworks such as pytorch and tensorflow, computer vision, nlp, or related areas would be a plus.instabase is an equal opportunity employer and values diversity in all forms. instabase does not discriminate on the basis of race, religion, color, national origin, gender identity, sexual orientation, age, marital status, protected veteran status, disability, or any other unlawful factor. instabase also complies with local laws, including the san francisco fair chance ordinance.</t>
+          <t>join us for a 12-week internship with the global reference lab information systems group.idexx reference laboratoriesis a global network united by a shared commitment to enhancing pet care where the true strength in our name is the people behind it. our reference laboratories make it possible for our customers to discover more with our unrelenting commitment to innovation, personalized support, guidance, and expertise while providing the most complete and advanced menu of diagnostic tests along with technology and tools.this team has software product management responsibility for the software applications used by laboratory technicians in our global network of reference laboratories.laboratory technicians within our reference labs use an ecosystem of applications consisting of a mix internally developed plus third party purchased software. thesoftware ecosystemfacilitates taking in the samples, checking them into the labs with sample management, routing the samples through the lab to complete the diagnostics and then sending the result back out to the customer. this team owns software product management for this ecosystem of applications.as software product management within the global reference lab information systems, we bridge the gap between what the users need, and we turn that into requirements and work with the technical teams to prioritize it and then realize it within the laboratory.in this internship role you would…contribute to putting in a regular, proactive patching program for our applications. to start this initiative, what we need is for you to create a catalogue of our applications, when they were last patched, and how many versions they are behind. work with stakeholders to identify maintenance windows when it is a good time to do the patch, and what frequency, etc.another aspect of this internship is to tour a reference laboratory, observe existing processes, and propose ways for new technology to enhance these processes. in this exploratory part of the internship, you would be looking at opportunities for automation, for example, to use voice recognition technology. tools like microsoft hololens are also available for this part of the internship. proposed technologies can include assisted intelligence and machine learning. we would look to you to come up with proposals for innovation.day-to-day asks are likely to includeworking on a patch program with it, software product managers, and business stakeholdersto catalogue one application, for instance, you would go talk to the product owner that is on the team about what the application does – the functionality and the architecture. then you would go to your contact within it to figure out what the patching strategy should be for it. from there you would figure out what we need to do to do the patch, when to schedule it, how frequently they happen, how out of date is it and what other systems does it impact if we go and patch this and not that, so looking at what is our testing and implementation strategy.there are 25+ points within the ecosystem to categorize. by the time you categorize it, you may realize you missed a data point, then go back and get the data point again, then go back to the business about what is realistic for uptime/downtime/when you are going to do the patch, can you coordinate it with the other systems. there are a lot of pieces to it, so we imagine it being very iterative.ideal skills for this role includeexcellent communication skills, willing to speak up and reach out to different people to get things done.knowledge of computer infrastructure, knowledge of systems architecture and application architecture are all helpful for this internshipbeing detail-oriented and organized, with the ability to pull together all the pieces involved in the projectrequirements for the role includecurrently enrolled in an undergraduate or graduate program majoring in computer science, information systems, network architecture, computer engineering, or other related technology majors.applicants must be at least 18 years of age and must have completed at least one year of college.a track record of student success and potential as demonstrated by gpa, research portfolio, prior work experiences and/or the recommendation of a professor preferred.what’s in it for youyou would get exposure to a corporate enterprise it environment and how systems work together and impact each other, and how you establish good governance and maintenance of those systems! you also would have the opportunity to explore implementing the latest technologies in a production laboratory environment.interns will also be invited to participate in an intern-only slate of programming that includes social/networking events.idexx values a diverse workforce and workplace and strongly encourages women, people of color, lgbt individuals, people with disabilities, members of ethnic minorities, foreign-born residents, and veterans to apply.idexx is an equal opportunity employer. applicants will not be discriminated against because of race, color, creed, sex, sexual orientation, gender identity or expression, age, religion, national origin, citizenship status, disability, ancestry, marital status, veteran status, medical condition, or any protected category prohibited by local, state, or federal laws.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>at instabase, we’re passionate about building software to advance the state of the art in computing. we’ve built a fearlessly experimental, customer-obsessed team who are making discoveries to fundamentally change how people build and consume business applications. today, we’re partnering with the world’s leading companies to transform how they use data and technology. if these challenges excite you, we’d love to hear from you!our engineering teamarchitects the underlying operating system, core services, platform infrastructure, dev toolkits, core algorithms, machine learning models, packaged end-user apps, and app store marketplace. instabase engineers are excited to solve hard problems for complex organizations and are self-starters from day one.what you will do:work on a small team of ml engineers to apply machine learning techniques to challenging real world problems such asimage processing / computer visionocrhandwriting recognitionvisual extraction (checkboxes, signatures, radio button, etc.)object detectiontable detectiondocument/text understandingextraction from documentsfield extraction from document with variable structure (for example: paystubs, invoices, forms, etc.)information retrieval from documents with natural languagefinding relevant clause in legal contractsextracting data (for example: effective date, duration, payment terms, etc.) from legal contractsdocument classificationdocument clusteringworking in this area require knowledge in one or more of the following:ms in computer science, engineering, math, science or related field. phd preferred.5+ years industry / academia experienceproven ttrack record of excellence in applying machine learning techniques for solving difficult real world problemsknowledge of deep learning frameworks such as pytorch and tensorflow, computer vision, nlp, or related areas would be a plus.instabase is an equal opportunity employer and values diversity in all forms. instabase does not discriminate on the basis of race, religion, color, national origin, gender identity, sexual orientation, age, marital status, protected veteran status, disability, or any other unlawful factor. instabase also complies with local laws, including the san francisco fair chance ordinance.</t>
+          <t>join us for a 12-week internship with the global reference lab information systems group.idexx reference laboratoriesis a global network united by a shared commitment to enhancing pet care where the true strength in our name is the people behind it. our reference laboratories make it possible for our customers to discover more with our unrelenting commitment to innovation, personalized support, guidance, and expertise while providing the most complete and advanced menu of diagnostic tests along with technology and tools.this team has software product management responsibility for the software applications used by laboratory technicians in our global network of reference laboratories.laboratory technicians within our reference labs use an ecosystem of applications consisting of a mix internally developed plus third party purchased software. thesoftware ecosystemfacilitates taking in the samples, checking them into the labs with sample management, routing the samples through the lab to complete the diagnostics and then sending the result back out to the customer. this team owns software product management for this ecosystem of applications.as software product management within the global reference lab information systems, we bridge the gap between what the users need, and we turn that into requirements and work with the technical teams to prioritize it and then realize it within the laboratory.in this internship role you would…contribute to putting in a regular, proactive patching program for our applications. to start this initiative, what we need is for you to create a catalogue of our applications, when they were last patched, and how many versions they are behind. work with stakeholders to identify maintenance windows when it is a good time to do the patch, and what frequency, etc.another aspect of this internship is to tour a reference laboratory, observe existing processes, and propose ways for new technology to enhance these processes. in this exploratory part of the internship, you would be looking at opportunities for automation, for example, to use voice recognition technology. tools like microsoft hololens are also available for this part of the internship. proposed technologies can include assisted intelligence and machine learning. we would look to you to come up with proposals for innovation.day-to-day asks are likely to includeworking on a patch program with it, software product managers, and business stakeholdersto catalogue one application, for instance, you would go talk to the product owner that is on the team about what the application does – the functionality and the architecture. then you would go to your contact within it to figure out what the patching strategy should be for it. from there you would figure out what we need to do to do the patch, when to schedule it, how frequently they happen, how out of date is it and what other systems does it impact if we go and patch this and not that, so looking at what is our testing and implementation strategy.there are 25+ points within the ecosystem to categorize. by the time you categorize it, you may realize you missed a data point, then go back and get the data point again, then go back to the business about what is realistic for uptime/downtime/when you are going to do the patch, can you coordinate it with the other systems. there are a lot of pieces to it, so we imagine it being very iterative.ideal skills for this role includeexcellent communication skills, willing to speak up and reach out to different people to get things done.knowledge of computer infrastructure, knowledge of systems architecture and application architecture are all helpful for this internshipbeing detail-oriented and organized, with the ability to pull together all the pieces involved in the projectrequirements for the role includecurrently enrolled in an undergraduate or graduate program majoring in computer science, information systems, network architecture, computer engineering, or other related technology majors.applicants must be at least 18 years of age and must have completed at least one year of college.a track record of student success and potential as demonstrated by gpa, research portfolio, prior work experiences and/or the recommendation of a professor preferred.what’s in it for youyou would get exposure to a corporate enterprise it environment and how systems work together and impact each other, and how you establish good governance and maintenance of those systems! you also would have the opportunity to explore implementing the latest technologies in a production laboratory environment.interns will also be invited to participate in an intern-only slate of programming that includes social/networking events.idexx values a diverse workforce and workplace and strongly encourages women, people of color, lgbt individuals, people with disabilities, members of ethnic minorities, foreign-born residents, and veterans to apply.idexx is an equal opportunity employer. applicants will not be discriminated against because of race, color, creed, sex, sexual orientation, gender identity or expression, age, religion, national origin, citizenship status, disability, ancestry, marital status, veteran status, medical condition, or any protected category prohibited by local, state, or federal laws.</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0.1270833333333334</v>
+        <v>0.1042272727272727</v>
       </c>
       <c r="H6" t="n">
-        <v>0.5035714285714287</v>
+        <v>0.364962703962704</v>
       </c>
       <c r="I6" t="inlineStr">
-        <is>
-          <t>['build', 'solve', 'apply', 'learn', '’re', 'advance', 'obsess', 'make', 'change', 'consume', 'partner', 'lead', 'transform', 'use', 'excite', 'love', 'hear', 'teamarchitect', 'underlie', 'package', 'do', 'work', 'challenge', 'visionocrhandwrite', 'languagefinde', 'contractsextracte', 'clusteringworke', 'require', 'follow', 'academia', 'relate', 'discriminate', 'protect', 'include']</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/3036847597</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Global Reference Lab Information Systems Intern</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>IDEXX</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>join us for a 12-week internship with the global reference lab information systems group.idexx reference laboratoriesis a global network united by a shared commitment to enhancing pet care where the true strength in our name is the people behind it. our reference laboratories make it possible for our customers to discover more with our unrelenting commitment to innovation, personalized support, guidance, and expertise while providing the most complete and advanced menu of diagnostic tests along with technology and tools.this team has software product management responsibility for the software applications used by laboratory technicians in our global network of reference laboratories.laboratory technicians within our reference labs use an ecosystem of applications consisting of a mix internally developed plus third party purchased software. thesoftware ecosystemfacilitates taking in the samples, checking them into the labs with sample management, routing the samples through the lab to complete the diagnostics and then sending the result back out to the customer. this team owns software product management for this ecosystem of applications.as software product management within the global reference lab information systems, we bridge the gap between what the users need, and we turn that into requirements and work with the technical teams to prioritize it and then realize it within the laboratory.in this internship role you would…contribute to putting in a regular, proactive patching program for our applications. to start this initiative, what we need is for you to create a catalogue of our applications, when they were last patched, and how many versions they are behind. work with stakeholders to identify maintenance windows when it is a good time to do the patch, and what frequency, etc.another aspect of this internship is to tour a reference laboratory, observe existing processes, and propose ways for new technology to enhance these processes. in this exploratory part of the internship, you would be looking at opportunities for automation, for example, to use voice recognition technology. tools like microsoft hololens are also available for this part of the internship. proposed technologies can include assisted intelligence and machine learning. we would look to you to come up with proposals for innovation.day-to-day asks are likely to includeworking on a patch program with it, software product managers, and business stakeholdersto catalogue one application, for instance, you would go talk to the product owner that is on the team about what the application does – the functionality and the architecture. then you would go to your contact within it to figure out what the patching strategy should be for it. from there you would figure out what we need to do to do the patch, when to schedule it, how frequently they happen, how out of date is it and what other systems does it impact if we go and patch this and not that, so looking at what is our testing and implementation strategy.there are 25+ points within the ecosystem to categorize. by the time you categorize it, you may realize you missed a data point, then go back and get the data point again, then go back to the business about what is realistic for uptime/downtime/when you are going to do the patch, can you coordinate it with the other systems. there are a lot of pieces to it, so we imagine it being very iterative.ideal skills for this role includeexcellent communication skills, willing to speak up and reach out to different people to get things done.knowledge of computer infrastructure, knowledge of systems architecture and application architecture are all helpful for this internshipbeing detail-oriented and organized, with the ability to pull together all the pieces involved in the projectrequirements for the role includecurrently enrolled in an undergraduate or graduate program majoring in computer science, information systems, network architecture, computer engineering, or other related technology majors.applicants must be at least 18 years of age and must have completed at least one year of college.a track record of student success and potential as demonstrated by gpa, research portfolio, prior work experiences and/or the recommendation of a professor preferred.what’s in it for youyou would get exposure to a corporate enterprise it environment and how systems work together and impact each other, and how you establish good governance and maintenance of those systems! you also would have the opportunity to explore implementing the latest technologies in a production laboratory environment.interns will also be invited to participate in an intern-only slate of programming that includes social/networking events.idexx values a diverse workforce and workplace and strongly encourages women, people of color, lgbt individuals, people with disabilities, members of ethnic minorities, foreign-born residents, and veterans to apply.idexx is an equal opportunity employer. applicants will not be discriminated against because of race, color, creed, sex, sexual orientation, gender identity or expression, age, religion, national origin, citizenship status, disability, ancestry, marital status, veteran status, medical condition, or any protected category prohibited by local, state, or federal laws.</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>join us for a 12-week internship with the global reference lab information systems group.idexx reference laboratoriesis a global network united by a shared commitment to enhancing pet care where the true strength in our name is the people behind it. our reference laboratories make it possible for our customers to discover more with our unrelenting commitment to innovation, personalized support, guidance, and expertise while providing the most complete and advanced menu of diagnostic tests along with technology and tools.this team has software product management responsibility for the software applications used by laboratory technicians in our global network of reference laboratories.laboratory technicians within our reference labs use an ecosystem of applications consisting of a mix internally developed plus third party purchased software. thesoftware ecosystemfacilitates taking in the samples, checking them into the labs with sample management, routing the samples through the lab to complete the diagnostics and then sending the result back out to the customer. this team owns software product management for this ecosystem of applications.as software product management within the global reference lab information systems, we bridge the gap between what the users need, and we turn that into requirements and work with the technical teams to prioritize it and then realize it within the laboratory.in this internship role you would…contribute to putting in a regular, proactive patching program for our applications. to start this initiative, what we need is for you to create a catalogue of our applications, when they were last patched, and how many versions they are behind. work with stakeholders to identify maintenance windows when it is a good time to do the patch, and what frequency, etc.another aspect of this internship is to tour a reference laboratory, observe existing processes, and propose ways for new technology to enhance these processes. in this exploratory part of the internship, you would be looking at opportunities for automation, for example, to use voice recognition technology. tools like microsoft hololens are also available for this part of the internship. proposed technologies can include assisted intelligence and machine learning. we would look to you to come up with proposals for innovation.day-to-day asks are likely to includeworking on a patch program with it, software product managers, and business stakeholdersto catalogue one application, for instance, you would go talk to the product owner that is on the team about what the application does – the functionality and the architecture. then you would go to your contact within it to figure out what the patching strategy should be for it. from there you would figure out what we need to do to do the patch, when to schedule it, how frequently they happen, how out of date is it and what other systems does it impact if we go and patch this and not that, so looking at what is our testing and implementation strategy.there are 25+ points within the ecosystem to categorize. by the time you categorize it, you may realize you missed a data point, then go back and get the data point again, then go back to the business about what is realistic for uptime/downtime/when you are going to do the patch, can you coordinate it with the other systems. there are a lot of pieces to it, so we imagine it being very iterative.ideal skills for this role includeexcellent communication skills, willing to speak up and reach out to different people to get things done.knowledge of computer infrastructure, knowledge of systems architecture and application architecture are all helpful for this internshipbeing detail-oriented and organized, with the ability to pull together all the pieces involved in the projectrequirements for the role includecurrently enrolled in an undergraduate or graduate program majoring in computer science, information systems, network architecture, computer engineering, or other related technology majors.applicants must be at least 18 years of age and must have completed at least one year of college.a track record of student success and potential as demonstrated by gpa, research portfolio, prior work experiences and/or the recommendation of a professor preferred.what’s in it for youyou would get exposure to a corporate enterprise it environment and how systems work together and impact each other, and how you establish good governance and maintenance of those systems! you also would have the opportunity to explore implementing the latest technologies in a production laboratory environment.interns will also be invited to participate in an intern-only slate of programming that includes social/networking events.idexx values a diverse workforce and workplace and strongly encourages women, people of color, lgbt individuals, people with disabilities, members of ethnic minorities, foreign-born residents, and veterans to apply.idexx is an equal opportunity employer. applicants will not be discriminated against because of race, color, creed, sex, sexual orientation, gender identity or expression, age, religion, national origin, citizenship status, disability, ancestry, marital status, veteran status, medical condition, or any protected category prohibited by local, state, or federal laws.</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>0.1042272727272727</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.364962703962704</v>
-      </c>
-      <c r="I7" t="inlineStr">
         <is>
           <t>['go', 'do', 'use', 'need', 'patch', 'look', 'get', 'enhance', 'have', 'complete', 'realize', 'propose', 'include', 'figure', 'impact', 'categorize', 'join', 'unite', 'share', 'make', 'discover', 'personalize', 'provide', 'consist', 'develop', 'purchase', 'ecosystemfacilitate', 'take', 'check', 'route', 'send', 'own', 'bridge', 'turn', 'prioritize', 'contribute', 'put', 'start', 'create', 'identify', 'tour', 'observe', 'exist', 'assist', 'come', 'includeworke', 'talk', 'schedule', 'happen', 'miss', 'coordinate', 'be', 'imagine', 'speak', 'reach', 'internshipbee', 'orient', 'organize', 'pull', 'involve', 'enrol', 'major', 'demonstrate', '’s', 'work', 'establish', 'explore', 'implement', 'invite', 'participate', 'network', 'encourage', 'bear', 'discriminate', 'protect', 'prohibit']</t>
         </is>

</xml_diff>

<commit_message>
adding new test file for logistics jobs
</commit_message>
<xml_diff>
--- a/job_data.xlsx
+++ b/job_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -650,33 +650,115 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Global Reference Lab Information Systems Intern</t>
+          <t>Data Science Manager</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>IDEXX</t>
+          <t>Deloitte</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>join us for a 12-week internship with the global reference lab information systems group.idexx reference laboratoriesis a global network united by a shared commitment to enhancing pet care where the true strength in our name is the people behind it. our reference laboratories make it possible for our customers to discover more with our unrelenting commitment to innovation, personalized support, guidance, and expertise while providing the most complete and advanced menu of diagnostic tests along with technology and tools.this team has software product management responsibility for the software applications used by laboratory technicians in our global network of reference laboratories.laboratory technicians within our reference labs use an ecosystem of applications consisting of a mix internally developed plus third party purchased software. thesoftware ecosystemfacilitates taking in the samples, checking them into the labs with sample management, routing the samples through the lab to complete the diagnostics and then sending the result back out to the customer. this team owns software product management for this ecosystem of applications.as software product management within the global reference lab information systems, we bridge the gap between what the users need, and we turn that into requirements and work with the technical teams to prioritize it and then realize it within the laboratory.in this internship role you would…contribute to putting in a regular, proactive patching program for our applications. to start this initiative, what we need is for you to create a catalogue of our applications, when they were last patched, and how many versions they are behind. work with stakeholders to identify maintenance windows when it is a good time to do the patch, and what frequency, etc.another aspect of this internship is to tour a reference laboratory, observe existing processes, and propose ways for new technology to enhance these processes. in this exploratory part of the internship, you would be looking at opportunities for automation, for example, to use voice recognition technology. tools like microsoft hololens are also available for this part of the internship. proposed technologies can include assisted intelligence and machine learning. we would look to you to come up with proposals for innovation.day-to-day asks are likely to includeworking on a patch program with it, software product managers, and business stakeholdersto catalogue one application, for instance, you would go talk to the product owner that is on the team about what the application does – the functionality and the architecture. then you would go to your contact within it to figure out what the patching strategy should be for it. from there you would figure out what we need to do to do the patch, when to schedule it, how frequently they happen, how out of date is it and what other systems does it impact if we go and patch this and not that, so looking at what is our testing and implementation strategy.there are 25+ points within the ecosystem to categorize. by the time you categorize it, you may realize you missed a data point, then go back and get the data point again, then go back to the business about what is realistic for uptime/downtime/when you are going to do the patch, can you coordinate it with the other systems. there are a lot of pieces to it, so we imagine it being very iterative.ideal skills for this role includeexcellent communication skills, willing to speak up and reach out to different people to get things done.knowledge of computer infrastructure, knowledge of systems architecture and application architecture are all helpful for this internshipbeing detail-oriented and organized, with the ability to pull together all the pieces involved in the projectrequirements for the role includecurrently enrolled in an undergraduate or graduate program majoring in computer science, information systems, network architecture, computer engineering, or other related technology majors.applicants must be at least 18 years of age and must have completed at least one year of college.a track record of student success and potential as demonstrated by gpa, research portfolio, prior work experiences and/or the recommendation of a professor preferred.what’s in it for youyou would get exposure to a corporate enterprise it environment and how systems work together and impact each other, and how you establish good governance and maintenance of those systems! you also would have the opportunity to explore implementing the latest technologies in a production laboratory environment.interns will also be invited to participate in an intern-only slate of programming that includes social/networking events.idexx values a diverse workforce and workplace and strongly encourages women, people of color, lgbt individuals, people with disabilities, members of ethnic minorities, foreign-born residents, and veterans to apply.idexx is an equal opportunity employer. applicants will not be discriminated against because of race, color, creed, sex, sexual orientation, gender identity or expression, age, religion, national origin, citizenship status, disability, ancestry, marital status, veteran status, medical condition, or any protected category prohibited by local, state, or federal laws.</t>
+          <t>do you have a passion for artificial intelligence, machine learning, and data analysis? do you yearn to have the impact of your work recognized and valued by more than just your development team? do you constantly wonder what you could build if only you had access to world-class data sets and computing resources?if yes, we have just the role for you.in deloitte's audit and assurance business, we make businesses and markets better. an audit is more than an obligation; it is an opportunity to see further and deeper into businesses. in our role as independent auditors, we enhance trust in the companies we audit, helping a multitrillion dollar capital markets system function with greater confidence. as we aspire to the very highest standards of audit quality, we deliver deeper insights that can help clients become more effective organizations.deloitte's audit and assurance business embraces the promise of artificial intelligence and machine learning, with various forms of ai and ml embedded in the audit technology solutions currently used by our 10,000+ practitioners today. within our dedicated data science organization, a subgroup of our award-winning audit transformation group, we continue that journey enabling the next generation of ai-enabled solutions that usher in a future that completely transforms the way our practitioners perform their audit work, and the insights we can provide to our clients.you will be joining a growing team of talented professionals in a fast-paced yet collaborative startup-like environment dedicated to realizing the deloitte audit and assurance vision of an ai-enabled audit. you will be leveraging the most advanced technologies in machine learning, natural language processing, time-series modeling, and reinforcement learning to lead our business into the future.as a data science manager, you will lead the technical and technological components of our data science workstreams and ai and ml solutions. you will work hand-in-hand with subject matter experts to ensure the inputs and outputs suit the intended user experience and audit workflow. you will manage data scientists, junior data scientists, and developers to complete the data science objectives that are required to fully develop and deploy a production-level ml solution. this includes performing or guiding research in an independent fashion, and interacting closely with key stakeholders with varying levels of machine learning experience.specifically, you will be expected to:have a profound understanding of the state of the art of a multitude of fields in artificial intelligence, including but not limited to nlp, probabilistic graphical models, time-series analysis, and weak supervised learning among otherslead the application of rigorous data science within your workstream, managing and supervising junior resources to do so; particularly:perform or lead the performance of exploratory data analysis to understand relationships and opportunities to influence outcomes, while being able to quickly iterate common feature transformation and model types to find the best predictive modelsdevelop and document proofs of concept to verify your ideas, including counterfactual explanations for interpretabilityclose the loop to make sure that the proposed solution is performing as it should and is correctly understoodcollaborate with subject matter experts to obtain a deep understanding of the underlying business problem, and to define and refine the corresponding technical solutionco-lead the planning and direction of a project with subject matter experts, and effectively prioritize goals and objectivesidentify opportunities to apply the latest advancements in machine learning and artificial intelligence to build, test, and validate predictive modelsmake impactful contributions to internal discussions on emerging machine learning methodologiesinfluence machine learning strategy for current and prospective workstreamsactively mentor data scientists and junior data scientists on good software practicesdevelop and embed automated processes for predictive model validation, deployment, and implementationarchitect ml pipelines and actively contribute high-quality, production-ready code (readable, well-tested, with well-designed apis)qualificationsrequired:phd in a quantitative field (computer science, engineering, mathematics, physics, machine learning, statistics)6+ years of industry experience leading the design, development, and deployment of machine learning modelsexperience being the technical lead for multiple project teams simultaneouslyprevious experience mentoring, training, and developing junior members of the team; experience in employee performance reviewsexpert understanding of python and other common languagesdeep understanding of machine learning model development life cyclesextensive experience using common machine learning and deep learning libraries and techniques, including tensorflow, pytorch, and big data platformsextensive experience with cloud-based ecosystems (azure, gcp, aws)experience in an agile working environment and related project management tools (jira, azure devops, etc.)demonstrated ability to write high-quality, production-ready code (readable, well-tested, well-documented, with well-designed apis)demonstrated ability to develop novel machine learning methods that go beyond putting together existing open-source code, and to apply problem-solving skills to complex issuesexperience with version control practices and tools (git, etc.)fluency in both structured and unstructured data (sql, nosql)solid understanding of docker, jenkins, kubernetes, and other devops toolsexcellent written and verbal communication skillsability to travel when necessarypreferred:10+ years of industry experience leading the design, development, and deployment of machine learning modelsprior scientific publication history. outstanding academic track record as evidenced by top tier publications.strong competency for additional coding languages (r, etc.)strong project management and delivery experience, including budget oversight and staffing of project teams including time managementextensive experience with microsoft azure, including certification in machine learningexperience with machine learning pipelines (azure ml)experience with ml ops and related governance processes, particularly within a regulated industrystrong presentation skills using microsoft office suite (visio, powerpoint, etc.)understanding of the capital markets, and the role public accounting firms</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>join us for a 12-week internship with the global reference lab information systems group.idexx reference laboratoriesis a global network united by a shared commitment to enhancing pet care where the true strength in our name is the people behind it. our reference laboratories make it possible for our customers to discover more with our unrelenting commitment to innovation, personalized support, guidance, and expertise while providing the most complete and advanced menu of diagnostic tests along with technology and tools.this team has software product management responsibility for the software applications used by laboratory technicians in our global network of reference laboratories.laboratory technicians within our reference labs use an ecosystem of applications consisting of a mix internally developed plus third party purchased software. thesoftware ecosystemfacilitates taking in the samples, checking them into the labs with sample management, routing the samples through the lab to complete the diagnostics and then sending the result back out to the customer. this team owns software product management for this ecosystem of applications.as software product management within the global reference lab information systems, we bridge the gap between what the users need, and we turn that into requirements and work with the technical teams to prioritize it and then realize it within the laboratory.in this internship role you would…contribute to putting in a regular, proactive patching program for our applications. to start this initiative, what we need is for you to create a catalogue of our applications, when they were last patched, and how many versions they are behind. work with stakeholders to identify maintenance windows when it is a good time to do the patch, and what frequency, etc.another aspect of this internship is to tour a reference laboratory, observe existing processes, and propose ways for new technology to enhance these processes. in this exploratory part of the internship, you would be looking at opportunities for automation, for example, to use voice recognition technology. tools like microsoft hololens are also available for this part of the internship. proposed technologies can include assisted intelligence and machine learning. we would look to you to come up with proposals for innovation.day-to-day asks are likely to includeworking on a patch program with it, software product managers, and business stakeholdersto catalogue one application, for instance, you would go talk to the product owner that is on the team about what the application does – the functionality and the architecture. then you would go to your contact within it to figure out what the patching strategy should be for it. from there you would figure out what we need to do to do the patch, when to schedule it, how frequently they happen, how out of date is it and what other systems does it impact if we go and patch this and not that, so looking at what is our testing and implementation strategy.there are 25+ points within the ecosystem to categorize. by the time you categorize it, you may realize you missed a data point, then go back and get the data point again, then go back to the business about what is realistic for uptime/downtime/when you are going to do the patch, can you coordinate it with the other systems. there are a lot of pieces to it, so we imagine it being very iterative.ideal skills for this role includeexcellent communication skills, willing to speak up and reach out to different people to get things done.knowledge of computer infrastructure, knowledge of systems architecture and application architecture are all helpful for this internshipbeing detail-oriented and organized, with the ability to pull together all the pieces involved in the projectrequirements for the role includecurrently enrolled in an undergraduate or graduate program majoring in computer science, information systems, network architecture, computer engineering, or other related technology majors.applicants must be at least 18 years of age and must have completed at least one year of college.a track record of student success and potential as demonstrated by gpa, research portfolio, prior work experiences and/or the recommendation of a professor preferred.what’s in it for youyou would get exposure to a corporate enterprise it environment and how systems work together and impact each other, and how you establish good governance and maintenance of those systems! you also would have the opportunity to explore implementing the latest technologies in a production laboratory environment.interns will also be invited to participate in an intern-only slate of programming that includes social/networking events.idexx values a diverse workforce and workplace and strongly encourages women, people of color, lgbt individuals, people with disabilities, members of ethnic minorities, foreign-born residents, and veterans to apply.idexx is an equal opportunity employer. applicants will not be discriminated against because of race, color, creed, sex, sexual orientation, gender identity or expression, age, religion, national origin, citizenship status, disability, ancestry, marital status, veteran status, medical condition, or any protected category prohibited by local, state, or federal laws.</t>
+          <t>do you have a passion for artificial intelligence, machine learning, and data analysis? do you yearn to have the impact of your work recognized and valued by more than just your development team? do you constantly wonder what you could build if only you had access to world-class data sets and computing resources?if yes, we have just the role for you.in deloitte's audit and assurance business, we make businesses and markets better. an audit is more than an obligation; it is an opportunity to see further and deeper into businesses. in our role as independent auditors, we enhance trust in the companies we audit, helping a multitrillion dollar capital markets system function with greater confidence. as we aspire to the very highest standards of audit quality, we deliver deeper insights that can help clients become more effective organizations.deloitte's audit and assurance business embraces the promise of artificial intelligence and machine learning, with various forms of ai and ml embedded in the audit technology solutions currently used by our 10,000+ practitioners today. within our dedicated data science organization, a subgroup of our award-winning audit transformation group, we continue that journey enabling the next generation of ai-enabled solutions that usher in a future that completely transforms the way our practitioners perform their audit work, and the insights we can provide to our clients.you will be joining a growing team of talented professionals in a fast-paced yet collaborative startup-like environment dedicated to realizing the deloitte audit and assurance vision of an ai-enabled audit. you will be leveraging the most advanced technologies in machine learning, natural language processing, time-series modeling, and reinforcement learning to lead our business into the future.as a data science manager, you will lead the technical and technological components of our data science workstreams and ai and ml solutions. you will work hand-in-hand with subject matter experts to ensure the inputs and outputs suit the intended user experience and audit workflow. you will manage data scientists, junior data scientists, and developers to complete the data science objectives that are required to fully develop and deploy a production-level ml solution. this includes performing or guiding research in an independent fashion, and interacting closely with key stakeholders with varying levels of machine learning experience.specifically, you will be expected to:have a profound understanding of the state of the art of a multitude of fields in artificial intelligence, including but not limited to nlp, probabilistic graphical models, time-series analysis, and weak supervised learning among otherslead the application of rigorous data science within your workstream, managing and supervising junior resources to do so; particularly:perform or lead the performance of exploratory data analysis to understand relationships and opportunities to influence outcomes, while being able to quickly iterate common feature transformation and model types to find the best predictive modelsdevelop and document proofs of concept to verify your ideas, including counterfactual explanations for interpretabilityclose the loop to make sure that the proposed solution is performing as it should and is correctly understoodcollaborate with subject matter experts to obtain a deep understanding of the underlying business problem, and to define and refine the corresponding technical solutionco-lead the planning and direction of a project with subject matter experts, and effectively prioritize goals and objectivesidentify opportunities to apply the latest advancements in machine learning and artificial intelligence to build, test, and validate predictive modelsmake impactful contributions to internal discussions on emerging machine learning methodologiesinfluence machine learning strategy for current and prospective workstreamsactively mentor data scientists and junior data scientists on good software practicesdevelop and embed automated processes for predictive model validation, deployment, and implementationarchitect ml pipelines and actively contribute high-quality, production-ready code (readable, well-tested, with well-designed apis)qualificationsrequired:phd in a quantitative field (computer science, engineering, mathematics, physics, machine learning, statistics)6+ years of industry experience leading the design, development, and deployment of machine learning modelsexperience being the technical lead for multiple project teams simultaneouslyprevious experience mentoring, training, and developing junior members of the team; experience in employee performance reviewsexpert understanding of python and other common languagesdeep understanding of machine learning model development life cyclesextensive experience using common machine learning and deep learning libraries and techniques, including tensorflow, pytorch, and big data platformsextensive experience with cloud-based ecosystems (azure, gcp, aws)experience in an agile working environment and related project management tools (jira, azure devops, etc.)demonstrated ability to write high-quality, production-ready code (readable, well-tested, well-documented, with well-designed apis)demonstrated ability to develop novel machine learning methods that go beyond putting together existing open-source code, and to apply problem-solving skills to complex issuesexperience with version control practices and tools (git, etc.)fluency in both structured and unstructured data (sql, nosql)solid understanding of docker, jenkins, kubernetes, and other devops toolsexcellent written and verbal communication skillsability to travel when necessarypreferred:10+ years of industry experience leading the design, development, and deployment of machine learning modelsprior scientific publication history. outstanding academic track record as evidenced by top tier publications.strong competency for additional coding languages (r, etc.)strong project management and delivery experience, including budget oversight and staffing of project teams including time managementextensive experience with microsoft azure, including certification in machine learningexperience with machine learning pipelines (azure ml)experience with ml ops and related governance processes, particularly within a regulated industrystrong presentation skills using microsoft office suite (visio, powerpoint, etc.)understanding of the capital markets, and the role public accounting firms</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0.1042272727272727</v>
+        <v>0.09478021978021978</v>
       </c>
       <c r="H6" t="n">
-        <v>0.364962703962704</v>
+        <v>0.4748473748473748</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>['go', 'do', 'use', 'need', 'patch', 'look', 'get', 'enhance', 'have', 'complete', 'realize', 'propose', 'include', 'figure', 'impact', 'categorize', 'join', 'unite', 'share', 'make', 'discover', 'personalize', 'provide', 'consist', 'develop', 'purchase', 'ecosystemfacilitate', 'take', 'check', 'route', 'send', 'own', 'bridge', 'turn', 'prioritize', 'contribute', 'put', 'start', 'create', 'identify', 'tour', 'observe', 'exist', 'assist', 'come', 'includeworke', 'talk', 'schedule', 'happen', 'miss', 'coordinate', 'be', 'imagine', 'speak', 'reach', 'internshipbee', 'orient', 'organize', 'pull', 'involve', 'enrol', 'major', 'demonstrate', '’s', 'work', 'establish', 'explore', 'implement', 'invite', 'participate', 'network', 'encourage', 'bear', 'discriminate', 'protect', 'prohibit']</t>
+          <t>['include', 'have', 'learn', 'lead', 'perform', 'use', 'enable', 'develop', 'build', 'make', 'help', 'work', 'manage', 'apply', 'test', 'design', 'write', 'yearn', 'recognize', 'value', 'wonder', 'see', 'enhance', 'audit', 'aspire', 'deliver', 'become', 'embrace', 'embed', 'win', 'continue', 'transform', 'provide', 'join', 'grow', 'pace', 'dedicate', 'realize', 'leverage', 'workstream', 'ai', 'ensure', 'suit', 'intend', 'complete', 'require', 'deploy', 'guide', 'interact', 'vary', 'expect', 'limit', 'supervise', 'do', 'understand', 'influence', 'iterate', 'find', 'verify', 'interpretabilityclose', 'propose', 'obtain', 'underlie', 'define', 'refine', 'correspond', 'prioritize', 'emerge', 'embe', 'automate', 'implementationarchitect', 'contribute', 'mentor', 'base', 'etc.)demonstrate', 'document', 'apis)demonstrate', 'go', 'put', 'exist', 'solve', 'travel', 'evidence', 'code', 'azure']</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/3036847597</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Entry Level Data Scientist</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>SynergisticIT</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>at synergisticit, we aim to bring aboard it professionals to help them build a rewarding career in cutting-edge technologies. being in the industry for more than 10 years, we provide a splendid range of lucrative opportunities to sustain a position in our top tech clients like google, apple, cognizant, client, paypal, to name a few. our seasoned team firmly believes that the new tech talent can scale any business if given the right opportunity. we value your integrity, hard work, and commitment to make a difference in the technical sphere. for this reason, we focus on providing end-to-end career assistance and enhancing your already existing it skills and knowledge. currently, we are looking for qualified entry-level data scientists who can apply data science principles to design, test, implement, and develop data-based solutions, including reporting, auditing, and preparing large databases for statistical analysis. minimum background and qualifications requirement bachelor's degree or master's degree in computer engineering, computer science, mathematics, electrical engineering, information systems, or it must have mathematics or statistics background technical and soft skills required experience in python programming and understanding of the software development life cycle. knowledge of linear algebra, statistics, and mathematics concepts. excellent written and verbal communication skills. highly motivated, self-learner, team player, and technically inquisitive. strong work ethics and creative problem-solving abilities. preferred skills deep learning data visualization nlp scala django roles and responsibilities collaborate with dynamic teams of engineers, developers, and scientists who research and integrate algorithms to develop an application, software, and computer system solutions to address complex data problems. assess project requirements and develop data analysis algorithms. engage developers to share their opinions, knowledge, and recommendations to meet the deliverables. contribute to technical solutions and implement software analyses to unlock the secrets held by big data sets. integrate components like web-based ui, commercial indexing products, and access control mechanisms to create operational information and knowledge discovery systems. benefits competitive salary flexible work schedule part-time off e-verified no relocation h1b filing on job technical support skill enhancement opportunity to work with fortune 500 companies who should apply? recent it graduates looking to build a solid career in the tech industry. if you're lured by the endless possibilities presented by ai, machine learning, iot, and data science, this job opportunity can be the right career path for you. candidate's outcome httpswww.synergisticit.comcandidate-outcomes httpswww.synergisticit.comcandidate-outcomes no third-party candidates or c2c candidates if you are interested, please apply to the posting. no phone calls please, shortlisted candidates would be reached out.</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>at synergisticit, we aim to bring aboard it professionals to help them build a rewarding career in cutting-edge technologies. being in the industry for more than 10 years, we provide a splendid range of lucrative opportunities to sustain a position in our top tech clients like google, apple, cognizant, client, paypal, to name a few. our seasoned team firmly believes that the new tech talent can scale any business if given the right opportunity. we value your integrity, hard work, and commitment to make a difference in the technical sphere. for this reason, we focus on providing end-to-end career assistance and enhancing your already existing it skills and knowledge. currently, we are looking for qualified entry-level data scientists who can apply data science principles to design, test, implement, and develop data-based solutions, including reporting, auditing, and preparing large databases for statistical analysis. minimum background and qualifications requirement bachelor's degree or master's degree in computer engineering, computer science, mathematics, electrical engineering, information systems, or it must have mathematics or statistics background technical and soft skills required experience in python programming and understanding of the software development life cycle. knowledge of linear algebra, statistics, and mathematics concepts. excellent written and verbal communication skills. highly motivated, self-learner, team player, and technically inquisitive. strong work ethics and creative problem-solving abilities. preferred skills deep learning data visualization nlp scala django roles and responsibilities collaborate with dynamic teams of engineers, developers, and scientists who research and integrate algorithms to develop an application, software, and computer system solutions to address complex data problems. assess project requirements and develop data analysis algorithms. engage developers to share their opinions, knowledge, and recommendations to meet the deliverables. contribute to technical solutions and implement software analyses to unlock the secrets held by big data sets. integrate components like web-based ui, commercial indexing products, and access control mechanisms to create operational information and knowledge discovery systems. benefits competitive salary flexible work schedule part-time off e-verified no relocation h1b filing on job technical support skill enhancement opportunity to work with fortune 500 companies who should apply? recent it graduates looking to build a solid career in the tech industry. if you're lured by the endless possibilities presented by ai, machine learning, iot, and data science, this job opportunity can be the right career path for you. candidate's outcome httpswww.synergisticit.comcandidate-outcomes httpswww.synergisticit.comcandidate-outcomes no third-party candidates or c2c candidates if you are interested, please apply to the posting. no phone calls please, shortlisted candidates would be reached out.</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>0.1510024350649351</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.4198816287878787</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>['apply', 'develop', 'build', 'provide', 'look', 'implement', 'base', 'integrate', 'aim', 'bring', 'help', 'cut', 'sustain', 'name', 'believe', 'scale', 'give', 'value', 'make', 'focus', 'enhance', 'exist', 'design', 'include', 'prepare', 'have', 'require', 'write', 'solve', 'learn', 'collaborate', 'research', 'address', 'assess', 'engage', 'share', 'meet', 'contribute', 'unlock', 'hold', 'create', 'benefit', '-', 'verify', 'file', 'work', 'graduate', 'lure', 'present', 'please', 'shortlist', 'reach']</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/3041899464</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Entry Level Data Scientist</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Dice</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>dice is the leading career destination for tech experts at every stage of their careers. our client, synergisticit, is seeking the following. apply via dice today!at synergisticit, we aim to bring aboard it professionals to help them build a rewarding career in cutting-edge technologies. being in the industry for more than 10 years, we provide a splendid range of lucrative opportunities to sustain a position in our top tech clients like google, apple, cognizant, client, paypal, to name a few. our seasoned team firmly believes that the new tech talent can scale any business if given the right opportunity. we value your integrity, hard work, and commitment to make a difference in the technical sphere. for this reason, we focus on providing end-to-end career assistance and enhancing your already existing it skills and knowledge. currently, we are looking for qualified entry-level data scientists who can apply data science principles to design, test, implement, and develop data-based solutions, including reporting, auditing, and preparing large databases for statistical analysis. minimum background and qualifications requirement bachelor's degree or master's degree in computer engineering, computer science, mathematics, electrical engineering, information systems, or it must have mathematics or statistics background technical and soft skills required experience in python programming and understanding of the software development life cycle. knowledge of linear algebra, statistics, and mathematics concepts. excellent written and verbal communication skills. highly motivated, self-learner, team player, and technically inquisitive. strong work ethics and creative problem-solving abilities. preferred skills deep learning data visualization nlp scala django roles and responsibilities collaborate with dynamic teams of engineers, developers, and scientists who research and integrate algorithms to develop an application, software, and computer system solutions to address complex data problems. assess project requirements and develop data analysis algorithms. engage developers to share their opinions, knowledge, and recommendations to meet the deliverables. contribute to technical solutions and implement software analyses to unlock the secrets held by big data sets. integrate components like web-based ui, commercial indexing products, and access control mechanisms to create operational information and knowledge discovery systems. benefits competitive salary flexible work schedule part-time off e-verified no relocation h1b filing on job technical support skill enhancement opportunity to work with fortune 500 companies who should apply? recent it graduates looking to build a solid career in the tech industry. if you're lured by the endless possibilities presented by ai, machine learning, iot, and data science, this job opportunity can be the right career path for you. candidate's outcome httpswww.synergisticit.comcandidate-outcomes httpswww.synergisticit.comcandidate-outcomes no third-party candidates or c2c candidates if you are interested, please apply to the posting. no phone calls please, shortlisted candidates would be reached out.</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>dice is the leading career destination for tech experts at every stage of their careers. our client, synergisticit, is seeking the following. apply via dice today!at synergisticit, we aim to bring aboard it professionals to help them build a rewarding career in cutting-edge technologies. being in the industry for more than 10 years, we provide a splendid range of lucrative opportunities to sustain a position in our top tech clients like google, apple, cognizant, client, paypal, to name a few. our seasoned team firmly believes that the new tech talent can scale any business if given the right opportunity. we value your integrity, hard work, and commitment to make a difference in the technical sphere. for this reason, we focus on providing end-to-end career assistance and enhancing your already existing it skills and knowledge. currently, we are looking for qualified entry-level data scientists who can apply data science principles to design, test, implement, and develop data-based solutions, including reporting, auditing, and preparing large databases for statistical analysis. minimum background and qualifications requirement bachelor's degree or master's degree in computer engineering, computer science, mathematics, electrical engineering, information systems, or it must have mathematics or statistics background technical and soft skills required experience in python programming and understanding of the software development life cycle. knowledge of linear algebra, statistics, and mathematics concepts. excellent written and verbal communication skills. highly motivated, self-learner, team player, and technically inquisitive. strong work ethics and creative problem-solving abilities. preferred skills deep learning data visualization nlp scala django roles and responsibilities collaborate with dynamic teams of engineers, developers, and scientists who research and integrate algorithms to develop an application, software, and computer system solutions to address complex data problems. assess project requirements and develop data analysis algorithms. engage developers to share their opinions, knowledge, and recommendations to meet the deliverables. contribute to technical solutions and implement software analyses to unlock the secrets held by big data sets. integrate components like web-based ui, commercial indexing products, and access control mechanisms to create operational information and knowledge discovery systems. benefits competitive salary flexible work schedule part-time off e-verified no relocation h1b filing on job technical support skill enhancement opportunity to work with fortune 500 companies who should apply? recent it graduates looking to build a solid career in the tech industry. if you're lured by the endless possibilities presented by ai, machine learning, iot, and data science, this job opportunity can be the right career path for you. candidate's outcome httpswww.synergisticit.comcandidate-outcomes httpswww.synergisticit.comcandidate-outcomes no third-party candidates or c2c candidates if you are interested, please apply to the posting. no phone calls please, shortlisted candidates would be reached out.</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>0.146426603699331</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.410188246097337</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>['apply', 'develop', 'build', 'provide', 'look', 'implement', 'base', 'integrate', 'lead', 'seek', 'aim', 'bring', 'help', 'cut', 'sustain', 'name', 'believe', 'scale', 'give', 'value', 'make', 'focus', 'enhance', 'exist', 'design', 'include', 'prepare', 'have', 'require', 'write', 'solve', 'learn', 'collaborate', 'research', 'address', 'assess', 'engage', 'share', 'meet', 'contribute', 'unlock', 'hold', 'create', 'benefit', '-', 'verify', 'file', 'work', 'graduate', 'lure', 'present', 'please', 'shortlist', 'reach']</t>
         </is>
       </c>
     </row>

</xml_diff>